<commit_message>
fix cargue de medidas masivamente
</commit_message>
<xml_diff>
--- a/Catalogos/FormatMeasurements.xlsx
+++ b/Catalogos/FormatMeasurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\Greenpack\htdocs\Catalogos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\greenpack\htdocs\Catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C19FBA0-9343-4408-9A69-DD5C1F52EF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D06D0C-A91D-4AF6-85E0-08660E9A77A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Largo</t>
   </si>
   <si>
-    <t>Ventana</t>
-  </si>
-  <si>
     <t>LargoUtil</t>
   </si>
   <si>
@@ -49,25 +46,41 @@
   </si>
   <si>
     <t>VentaMinimaGenerica</t>
+  </si>
+  <si>
+    <t>Referencia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -82,8 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,35 +420,35 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>